<commit_message>
adding udemy data analytics - 2782024
</commit_message>
<xml_diff>
--- a/UdemyDataAnalytics/ClassicModelDataAnalysis_Udemy/udemy_02_SalesOverviewByCountry/CMDA_udemy_02_SalesOverviewByCountry.xlsx
+++ b/UdemyDataAnalytics/ClassicModelDataAnalysis_Udemy/udemy_02_SalesOverviewByCountry/CMDA_udemy_02_SalesOverviewByCountry.xlsx
@@ -8,25 +8,64 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RECYCLE BIN EXTRAS\ONLY_DOCS\MyProjectsForFun\UdemyDataAnalytics\ClassicModelDataAnalysis_Udemy\udemy_02_SalesOverviewByCountry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D11001-F242-41B3-95BF-07D672910F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A93AC7-37E7-4DEB-89C7-3BB0CD1D8E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SalesOverviewByCountry" sheetId="7" r:id="rId1"/>
-    <sheet name="CountryOverview" sheetId="6" r:id="rId2"/>
+    <sheet name="CountryOverview1" sheetId="8" r:id="rId2"/>
+    <sheet name="CountryOverview2" sheetId="9" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SalesOverviewByCountry!$A$1:$K$1422</definedName>
+    <definedName name="_xlcn.WorksheetConnection_SalesOverviewByCountryA1K14221" hidden="1">SalesOverviewByCountry!$A$1:$K$1422</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="16" r:id="rId5"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="Range" name="Range" connection="WorksheetConnection_SalesOverviewByCountry!$A$1:$K$1422"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{2EA8195E-11DF-4AC2-A59E-9623B890469C}" keepAlive="1" name="ThisWorkbookDataModel" description="Data Model" type="5" refreshedVersion="8" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" xr16:uid="{F099FF27-BF61-46C5-BB70-249F2D2BB584}" name="WorksheetConnection_SalesOverviewByCountry!$A$1:$K$1422" type="102" refreshedVersion="8" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="Range" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_SalesOverviewByCountryA1K14221"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4274" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4420" uniqueCount="118">
   <si>
     <t>orderDate</t>
   </si>
@@ -357,13 +396,38 @@
   <si>
     <t>Chatswood</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of Sales Value</t>
+  </si>
+  <si>
+    <t>Sum of Net Profit</t>
+  </si>
+  <si>
+    <t>% Net Profit</t>
+  </si>
+  <si>
+    <t>Sales_value</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -406,11 +470,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -430,12 +495,82 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -446,6 +581,1762 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CountryOverview2!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sales Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountryOverview2!$Q$4:$Q$23</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>New Zealand</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Singapore</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Finland</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountryOverview2!$R$4:$R$23</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>18045347479</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32678879418</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53876342276</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12609343238</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63940286484</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16451733640</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29125960088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13706674673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16126993256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25608235017</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>186287017892</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9016752012</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22414795375</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12988730132</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4746377142</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1582845240</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6254640854</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12233360052</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8627605479</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12130732141</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2027-4D9F-AEEA-4EE2F148F314}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="2031042176"/>
+        <c:axId val="2031042656"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CountryOverview2!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% Net Profit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>CountryOverview2!$Q$4:$Q$23</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>UK</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Norway</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>New Zealand</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Singapore</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Denmark</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Austria</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Philippines</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ireland</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Finland</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>CountryOverview2!$S$4:$S$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.9918546835919313</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9915727521177391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99149112957833041</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99142796608198736</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99134369079221285</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99133099238166367</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99127834596687991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99127133097091202</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99120948894318794</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99112151660436321</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99111574758285359</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99106562181783553</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99079899235662772</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99071411790573338</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99067171505226337</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99066360116166507</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.9903923470439443</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99038319150585563</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99024328504880166</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.98995618290933962</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2027-4D9F-AEEA-4EE2F148F314}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2031064256"/>
+        <c:axId val="2031050816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2031042176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2031042656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2031042656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2031042176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2031050816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2031064256"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="2031064256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2031050816"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>40820</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>48078</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>371928</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>154213</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{397BEF9E-304F-12AA-20D2-827F47C329D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Manoj Deshpande" refreshedDate="45529.91758252315" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{27147490-F97C-47AE-B5D8-676818480838}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="3">
+    <cacheField name="[Range].[country].[country]" caption="country" numFmtId="0" hierarchy="7" level="1">
+      <sharedItems count="20">
+        <s v="Australia"/>
+        <s v="Austria"/>
+        <s v="Belgium"/>
+        <s v="Canada"/>
+        <s v="Denmark"/>
+        <s v="Finland"/>
+        <s v="France"/>
+        <s v="Germany"/>
+        <s v="Ireland"/>
+        <s v="Italy"/>
+        <s v="Japan"/>
+        <s v="New Zealand"/>
+        <s v="Norway"/>
+        <s v="Philippines"/>
+        <s v="Singapore"/>
+        <s v="Spain"/>
+        <s v="Sweden"/>
+        <s v="Switzerland"/>
+        <s v="UK"/>
+        <s v="USA"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Sum of Sales Value]" caption="Sum of Sales Value" numFmtId="0" hierarchy="13" level="32767"/>
+    <cacheField name="[Measures].[Sum of Net Profit]" caption="Sum of Net Profit" numFmtId="0" hierarchy="14" level="32767"/>
+  </cacheFields>
+  <cacheHierarchies count="15">
+    <cacheHierarchy uniqueName="[Range].[orderDate]" caption="orderDate" attribute="1" time="1" defaultMemberUniqueName="[Range].[orderDate].[All]" allUniqueName="[Range].[orderDate].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[orderNumber]" caption="orderNumber" attribute="1" defaultMemberUniqueName="[Range].[orderNumber].[All]" allUniqueName="[Range].[orderNumber].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[quantityOrdered]" caption="quantityOrdered" attribute="1" defaultMemberUniqueName="[Range].[quantityOrdered].[All]" allUniqueName="[Range].[quantityOrdered].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[priceeach]" caption="priceeach" attribute="1" defaultMemberUniqueName="[Range].[priceeach].[All]" allUniqueName="[Range].[priceeach].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[productline]" caption="productline" attribute="1" defaultMemberUniqueName="[Range].[productline].[All]" allUniqueName="[Range].[productline].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[buyprice]" caption="buyprice" attribute="1" defaultMemberUniqueName="[Range].[buyprice].[All]" allUniqueName="[Range].[buyprice].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[city]" caption="city" attribute="1" defaultMemberUniqueName="[Range].[city].[All]" allUniqueName="[Range].[city].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[country]" caption="country" attribute="1" defaultMemberUniqueName="[Range].[country].[All]" allUniqueName="[Range].[country].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Range].[Sales Value]" caption="Sales Value" attribute="1" defaultMemberUniqueName="[Range].[Sales Value].[All]" allUniqueName="[Range].[Sales Value].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Cost Of sales]" caption="Cost Of sales" attribute="1" defaultMemberUniqueName="[Range].[Cost Of sales].[All]" allUniqueName="[Range].[Cost Of sales].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Net Profit]" caption="Net Profit" attribute="1" defaultMemberUniqueName="[Range].[Net Profit].[All]" allUniqueName="[Range].[Net Profit].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Range]" caption="__XL_Count Range" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Sales Value]" caption="Sum of Sales Value" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Net Profit]" caption="Sum of Net Profit" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="10"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Range" uniqueName="[Range]" caption="Range"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Range" caption="Range"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Manoj Deshpande" refreshedDate="45529.91758252315" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{D5C53CAB-60C3-4818-9A5C-2C6718FEBA3F}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="3">
+    <cacheField name="[Range].[country].[country]" caption="country" numFmtId="0" hierarchy="7" level="1">
+      <sharedItems count="20">
+        <s v="Australia"/>
+        <s v="Austria"/>
+        <s v="Belgium"/>
+        <s v="Canada"/>
+        <s v="Denmark"/>
+        <s v="Finland"/>
+        <s v="France"/>
+        <s v="Germany"/>
+        <s v="Ireland"/>
+        <s v="Italy"/>
+        <s v="Japan"/>
+        <s v="New Zealand"/>
+        <s v="Norway"/>
+        <s v="Philippines"/>
+        <s v="Singapore"/>
+        <s v="Spain"/>
+        <s v="Sweden"/>
+        <s v="Switzerland"/>
+        <s v="UK"/>
+        <s v="USA"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Sum of Sales Value]" caption="Sum of Sales Value" numFmtId="0" hierarchy="13" level="32767"/>
+    <cacheField name="[Measures].[Sum of Net Profit]" caption="Sum of Net Profit" numFmtId="0" hierarchy="14" level="32767"/>
+  </cacheFields>
+  <cacheHierarchies count="15">
+    <cacheHierarchy uniqueName="[Range].[orderDate]" caption="orderDate" attribute="1" time="1" defaultMemberUniqueName="[Range].[orderDate].[All]" allUniqueName="[Range].[orderDate].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="7" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[orderNumber]" caption="orderNumber" attribute="1" defaultMemberUniqueName="[Range].[orderNumber].[All]" allUniqueName="[Range].[orderNumber].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[quantityOrdered]" caption="quantityOrdered" attribute="1" defaultMemberUniqueName="[Range].[quantityOrdered].[All]" allUniqueName="[Range].[quantityOrdered].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[priceeach]" caption="priceeach" attribute="1" defaultMemberUniqueName="[Range].[priceeach].[All]" allUniqueName="[Range].[priceeach].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[productline]" caption="productline" attribute="1" defaultMemberUniqueName="[Range].[productline].[All]" allUniqueName="[Range].[productline].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[buyprice]" caption="buyprice" attribute="1" defaultMemberUniqueName="[Range].[buyprice].[All]" allUniqueName="[Range].[buyprice].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[city]" caption="city" attribute="1" defaultMemberUniqueName="[Range].[city].[All]" allUniqueName="[Range].[city].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[country]" caption="country" attribute="1" defaultMemberUniqueName="[Range].[country].[All]" allUniqueName="[Range].[country].[All]" dimensionUniqueName="[Range]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Range].[Sales Value]" caption="Sales Value" attribute="1" defaultMemberUniqueName="[Range].[Sales Value].[All]" allUniqueName="[Range].[Sales Value].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Cost Of sales]" caption="Cost Of sales" attribute="1" defaultMemberUniqueName="[Range].[Cost Of sales].[All]" allUniqueName="[Range].[Cost Of sales].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Range].[Net Profit]" caption="Net Profit" attribute="1" defaultMemberUniqueName="[Range].[Net Profit].[All]" allUniqueName="[Range].[Net Profit].[All]" dimensionUniqueName="[Range]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count Range]" caption="__XL_Count Range" measure="1" displayFolder="" measureGroup="Range" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Sales Value]" caption="Sum of Sales Value" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="8"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Net Profit]" caption="Sum of Net Profit" measure="1" displayFolder="" measureGroup="Range" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="10"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Range" uniqueName="[Range]" caption="Range"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Range" caption="Range"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8CD81EE0-5C69-4B1E-85E6-E9E7DC54B9D7}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C24" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Sales Value" fld="1" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Sum of Net Profit" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="10">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotHierarchies count="15">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="7"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_SalesOverviewByCountry!$A$1:$K$1422">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BF714881-8C1C-450E-ABC8-34E6DBD7A3AC}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C24" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="21">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Sales Value" fld="1" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Sum of Net Profit" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotHierarchies count="15">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="1">
+    <rowHierarchyUsage hierarchyUsage="7"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="-2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_SalesOverviewByCountry!$A$1:$K$1422">
+        <x15:activeTabTopLevelEntity name="[Range]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{79CF303D-2490-4D90-9A4F-79A384C780FF}" name="Table1" displayName="Table1" ref="O3:Q23" totalsRowShown="0">
+  <autoFilter ref="O3:Q23" xr:uid="{79CF303D-2490-4D90-9A4F-79A384C780FF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{265D565F-9338-4AA4-959D-96BC89260207}" name="Country" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{A05A0018-CD62-44D2-A14C-BF84D0FF6A8E}" name="Sales Value" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{EB63B947-0BC0-4188-A240-2150F548AC3B}" name="% Net Profit" dataDxfId="4" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9850589B-185C-4F20-82DE-7182F9BDF0AE}" name="Table13" displayName="Table13" ref="Q3:S23" totalsRowShown="0">
+  <autoFilter ref="Q3:S23" xr:uid="{79CF303D-2490-4D90-9A4F-79A384C780FF}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Q4:S23">
+    <sortCondition descending="1" ref="S3:S23"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2C925B40-5CF4-4BE0-8110-9FBFBD9F3020}" name="Country" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1F15D919-853E-4EC2-8C4C-0C9B37B7A1F9}" name="Sales Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{9422EE50-B2F2-47D5-85CC-49944707023D}" name="% Net Profit" dataDxfId="0" dataCellStyle="Percent"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -713,8 +2604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CDB21B-ADBD-45DA-AE30-30BEC83132EC}">
   <dimension ref="A1:O1422"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,7 +2660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>37995</v>
       </c>
@@ -807,7 +2698,7 @@
         <v>382982001</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>37995</v>
       </c>
@@ -845,7 +2736,7 @@
         <v>384753327.89999998</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>37995</v>
       </c>
@@ -883,7 +2774,7 @@
         <v>384190242</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>37995</v>
       </c>
@@ -921,7 +2812,7 @@
         <v>385366187.25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>37995</v>
       </c>
@@ -959,7 +2850,7 @@
         <v>385742337.75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>37995</v>
       </c>
@@ -997,7 +2888,7 @@
         <v>384863893.35000002</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>37995</v>
       </c>
@@ -1035,7 +2926,7 @@
         <v>384451647.60000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>37995</v>
       </c>
@@ -1073,7 +2964,7 @@
         <v>386211576</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>38015</v>
       </c>
@@ -1111,7 +3002,7 @@
         <v>380502399.05000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>38015</v>
       </c>
@@ -1149,7 +3040,7 @@
         <v>384508799.89999998</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>38015</v>
       </c>
@@ -1187,7 +3078,7 @@
         <v>384807977.94999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>38015</v>
       </c>
@@ -1225,7 +3116,7 @@
         <v>386273836.35000002</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>38015</v>
       </c>
@@ -1263,7 +3154,7 @@
         <v>384625886.10000002</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>38015</v>
       </c>
@@ -1301,7 +3192,7 @@
         <v>386186401.85000002</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>38015</v>
       </c>
@@ -31002,7 +32893,7 @@
         <v>58</v>
       </c>
       <c r="H797" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I797" s="6">
         <f t="shared" si="36"/>
@@ -31040,7 +32931,7 @@
         <v>58</v>
       </c>
       <c r="H798" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I798" s="6">
         <f t="shared" si="36"/>
@@ -31078,7 +32969,7 @@
         <v>58</v>
       </c>
       <c r="H799" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I799" s="6">
         <f t="shared" si="36"/>
@@ -31116,7 +33007,7 @@
         <v>58</v>
       </c>
       <c r="H800" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I800" s="6">
         <f t="shared" si="36"/>
@@ -31154,7 +33045,7 @@
         <v>58</v>
       </c>
       <c r="H801" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I801" s="6">
         <f t="shared" si="36"/>
@@ -31192,7 +33083,7 @@
         <v>58</v>
       </c>
       <c r="H802" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I802" s="6">
         <f t="shared" si="36"/>
@@ -31230,7 +33121,7 @@
         <v>58</v>
       </c>
       <c r="H803" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I803" s="6">
         <f t="shared" si="36"/>
@@ -31268,7 +33159,7 @@
         <v>58</v>
       </c>
       <c r="H804" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I804" s="6">
         <f t="shared" si="36"/>
@@ -31306,7 +33197,7 @@
         <v>58</v>
       </c>
       <c r="H805" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I805" s="6">
         <f t="shared" si="36"/>
@@ -31344,7 +33235,7 @@
         <v>58</v>
       </c>
       <c r="H806" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I806" s="6">
         <f t="shared" si="36"/>
@@ -31382,7 +33273,7 @@
         <v>58</v>
       </c>
       <c r="H807" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I807" s="6">
         <f t="shared" si="36"/>
@@ -31420,7 +33311,7 @@
         <v>58</v>
       </c>
       <c r="H808" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I808" s="6">
         <f t="shared" si="36"/>
@@ -31458,7 +33349,7 @@
         <v>58</v>
       </c>
       <c r="H809" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I809" s="6">
         <f t="shared" si="36"/>
@@ -31496,7 +33387,7 @@
         <v>60</v>
       </c>
       <c r="H810" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I810" s="6">
         <f t="shared" si="36"/>
@@ -31534,7 +33425,7 @@
         <v>60</v>
       </c>
       <c r="H811" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I811" s="6">
         <f t="shared" si="36"/>
@@ -31572,7 +33463,7 @@
         <v>60</v>
       </c>
       <c r="H812" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I812" s="6">
         <f t="shared" si="36"/>
@@ -31610,7 +33501,7 @@
         <v>60</v>
       </c>
       <c r="H813" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I813" s="6">
         <f t="shared" si="36"/>
@@ -54774,15 +56665,1509 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8004187-C7BD-4D21-B35D-A20786C4F302}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE5459D-A0A5-4766-B964-59B2F6500C4E}">
+  <dimension ref="A3:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" t="s">
+        <v>114</v>
+      </c>
+      <c r="O3" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="C4" s="8">
+        <v>25380872727.610001</v>
+      </c>
+      <c r="D4" s="9">
+        <f>C4/B4</f>
+        <v>0.99112151660436321</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.99112151660436298</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0.99112151660436321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4702101583.5500002</v>
+      </c>
+      <c r="D5" s="9">
+        <f>C5/B5</f>
+        <v>0.99067171505226337</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.99067171505226337</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.99067171505226337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="C6" s="8">
+        <v>8936192939.5499992</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" ref="D5:D25" si="0">C6/B6</f>
+        <v>0.99106562181783553</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.99106562181783553</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P6" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.99106562181783553</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="C7" s="8">
+        <v>17898362414.09</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9918546835919313</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.9918546835919313</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="P7" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.9918546835919313</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12868118315.440001</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99071411790573338</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.99071411790573338</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P8" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.99071411790573338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="C9" s="8">
+        <v>8543428391.6300001</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99024328504880166</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.99024328504880166</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P9" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.99024328504880166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="C10" s="8">
+        <v>63386799593.360001</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99134369079221285</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0.99134369079221285</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P10" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.99134369079221285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="C11" s="8">
+        <v>15985228743.469999</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99120948894318794</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.99120948894318794</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="P11" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.99120948894318794</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6194548435.3100004</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9903923470439443</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.9903923470439443</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="P12" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0.9903923470439443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="C13" s="8">
+        <v>22208556671.43</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99079899235662772</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.99079899235662772</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.99079899235662772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="C14" s="8">
+        <v>16309113435.74</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99133099238166367</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.99133099238166367</v>
+      </c>
+      <c r="N14" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.99133099238166367</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="C15" s="8">
+        <v>28871933540.73</v>
+      </c>
+      <c r="D15" s="9">
+        <f>C15/B15</f>
+        <v>0.99127834596687991</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.99127834596687991</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P15" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.99127834596687991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8">
+        <v>12609343238</v>
+      </c>
+      <c r="C16" s="8">
+        <v>12501255520.08</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99142796608198736</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5926117650</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.99018229952792114</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P16" s="8">
+        <v>12609343238</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.99142796608198736</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1568067165.54</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99066360116166507</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="8">
+        <v>6683225588</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.99253251753769767</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0.99066360116166507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="C18" s="8">
+        <v>13587033646.290001</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99127133097091202</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.99066360116166507</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P18" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.99127133097091202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="C19" s="8">
+        <v>53417915460.779999</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99149112957833041</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.99127133097091202</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.99149112957833041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="C20" s="8">
+        <v>12115714171.139999</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99038319150585563</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.99149112957833041</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P20" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.99038319150585563</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="C21" s="8">
+        <v>12008893286.200001</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.98995618290933962</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.99038319150585563</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P21" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.98995618290933962</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="C22" s="8">
+        <v>32403486400.630001</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9915727521177391</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.98995618290933962</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P22" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0.9915727521177391</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="C23" s="8">
+        <v>184631997003.01001</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99111574758285359</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.9915727521177391</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="Q23" s="9">
+        <v>0.99111574758285359</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="8">
+        <v>558452651888</v>
+      </c>
+      <c r="C24" s="8">
+        <v>553519619445.57996</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99116660575298088</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.99111574758285359</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366051E2-F167-4448-9599-2ACAE1E472AA}">
+  <dimension ref="A3:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AC29" sqref="AC29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>116</v>
+      </c>
+      <c r="R3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="C4" s="8">
+        <v>25380872727.610001</v>
+      </c>
+      <c r="D4" s="9">
+        <f>C4/B4</f>
+        <v>0.99112151660436321</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.99112151660436298</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0.9918546835919313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4702101583.5500002</v>
+      </c>
+      <c r="D5" s="9">
+        <f>C5/B5</f>
+        <v>0.99067171505226337</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.99067171505226337</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="S5" s="9">
+        <v>0.9915727521177391</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="C6" s="8">
+        <v>8936192939.5499992</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" ref="D6:D24" si="0">C6/B6</f>
+        <v>0.99106562181783553</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.99106562181783553</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R6" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="S6" s="9">
+        <v>0.99149112957833041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="C7" s="8">
+        <v>17898362414.09</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9918546835919313</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="8">
+        <v>18045347479</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.9918546835919313</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" s="8">
+        <v>12609343238</v>
+      </c>
+      <c r="S7" s="9">
+        <v>0.99142796608198736</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12868118315.440001</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99071411790573338</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.99071411790573338</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R8" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="S8" s="9">
+        <v>0.99134369079221285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="C9" s="8">
+        <v>8543428391.6300001</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99024328504880166</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I9" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.99024328504880166</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R9" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="S9" s="9">
+        <v>0.99133099238166367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="C10" s="8">
+        <v>63386799593.360001</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99134369079221285</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="8">
+        <v>63940286484</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0.99134369079221285</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R10" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="S10" s="9">
+        <v>0.99127834596687991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="C11" s="8">
+        <v>15985228743.469999</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99120948894318794</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.99120948894318794</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R11" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="S11" s="9">
+        <v>0.99127133097091202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6194548435.3100004</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9903923470439443</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.9903923470439443</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="8">
+        <v>16126993256</v>
+      </c>
+      <c r="S12" s="9">
+        <v>0.99120948894318794</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="C13" s="8">
+        <v>22208556671.43</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99079899235662772</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.99079899235662772</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R13" s="8">
+        <v>25608235017</v>
+      </c>
+      <c r="S13" s="9">
+        <v>0.99112151660436321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="C14" s="8">
+        <v>16309113435.74</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99133099238166367</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="8">
+        <v>16451733640</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.99133099238166367</v>
+      </c>
+      <c r="N14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="S14" s="9">
+        <v>0.99111574758285359</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="C15" s="8">
+        <v>28871933540.73</v>
+      </c>
+      <c r="D15" s="9">
+        <f>C15/B15</f>
+        <v>0.99127834596687991</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" s="8">
+        <v>29125960088</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.99127834596687991</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R15" s="8">
+        <v>9016752012</v>
+      </c>
+      <c r="S15" s="9">
+        <v>0.99106562181783553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="8">
+        <v>12609343238</v>
+      </c>
+      <c r="C16" s="8">
+        <v>12501255520.08</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99142796608198736</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="8">
+        <v>5926117650</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.99018229952792114</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R16" s="8">
+        <v>22414795375</v>
+      </c>
+      <c r="S16" s="9">
+        <v>0.99079899235662772</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1568067165.54</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99066360116166507</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="8">
+        <v>6683225588</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.99253251753769767</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R17" s="8">
+        <v>12988730132</v>
+      </c>
+      <c r="S17" s="9">
+        <v>0.99071411790573338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="C18" s="8">
+        <v>13587033646.290001</v>
+      </c>
+      <c r="D18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99127133097091202</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.99066360116166507</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R18" s="8">
+        <v>4746377142</v>
+      </c>
+      <c r="S18" s="9">
+        <v>0.99067171505226337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="C19" s="8">
+        <v>53417915460.779999</v>
+      </c>
+      <c r="D19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99149112957833041</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="8">
+        <v>13706674673</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.99127133097091202</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R19" s="8">
+        <v>1582845240</v>
+      </c>
+      <c r="S19" s="9">
+        <v>0.99066360116166507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="C20" s="8">
+        <v>12115714171.139999</v>
+      </c>
+      <c r="D20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99038319150585563</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="8">
+        <v>53876342276</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.99149112957833041</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="R20" s="8">
+        <v>6254640854</v>
+      </c>
+      <c r="S20" s="9">
+        <v>0.9903923470439443</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="C21" s="8">
+        <v>12008893286.200001</v>
+      </c>
+      <c r="D21" s="9">
+        <f t="shared" si="0"/>
+        <v>0.98995618290933962</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.99038319150585563</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R21" s="8">
+        <v>12233360052</v>
+      </c>
+      <c r="S21" s="9">
+        <v>0.99038319150585563</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="C22" s="8">
+        <v>32403486400.630001</v>
+      </c>
+      <c r="D22" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9915727521177391</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I22" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.98995618290933962</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="R22" s="8">
+        <v>8627605479</v>
+      </c>
+      <c r="S22" s="9">
+        <v>0.99024328504880166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="C23" s="8">
+        <v>184631997003.01001</v>
+      </c>
+      <c r="D23" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99111574758285359</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="8">
+        <v>32678879418</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.9915727521177391</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R23" s="8">
+        <v>12130732141</v>
+      </c>
+      <c r="S23" s="9">
+        <v>0.98995618290933962</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="8">
+        <v>558452651888</v>
+      </c>
+      <c r="C24" s="8">
+        <v>553519619445.57996</v>
+      </c>
+      <c r="D24" s="9">
+        <f t="shared" si="0"/>
+        <v>0.99116660575298088</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="8">
+        <v>186287017892</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.99111574758285359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>